<commit_message>
Finish add skill feature testing
</commit_message>
<xml_diff>
--- a/AutomationTesting/src/main/resources/dataset.xlsx
+++ b/AutomationTesting/src/main/resources/dataset.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="addLeaveTypeTest" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="addSkillTest" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
   <si>
     <t xml:space="preserve">Testcase ID</t>
   </si>
@@ -96,6 +97,147 @@
   </si>
   <si>
     <t xml:space="preserve">ADD_LEAVE_TYPE_TC010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD_LEAVE_TYPE_TC011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorem ipsum dolor sit amet, 
+consectetur adipiscing elit. 
+Proin varius, neque a finibus consequat, 
+nulla neque gravida ipsum, a vulputate lectus turpis at nisl. 
+Nunc eget purus vitae nisl auctor consequat. 
+Donec cursus, ex at ultricies fringilla, urna quam consectetur lorem, 
+vel tincidunt ligula magna at ipsum. Fusce eu orci in erat tempus 
+mattis a eu libero. Etiam lacinia tincidunt sollicitudin. 
+Aliquam non metus lacinia, tristique libero vitae, congue augue. 
+Nunc accumsan cursus justo nec sollicitudin. Nunc porta velit in 
+lectus congue mattis. Cras nec metus volutpat, scelerisque mauris ac, lacinia metus. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error path: Insert an leave name with too long name
+- “Should not exceed 50 characters” error text pop out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skill name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skill description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD_SKILL_TC000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scheduling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Having ability to schedule for tasks up to 6 months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Happy path:
+- Skill is saved to database
+- Success message pop out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD_SKILL_TC001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Having ability to slide design and presentation with fluently by Vietnamese and English </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD_SKILL_TC002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questioning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Having ability to analyze the problem for asking the non-obvious question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD_SKILL_TC003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Having ability to use Java 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD_SKILL_TC004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error path: Insert an already existed skill name
+- “Already existed” error text pop out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD_SKILL_TC005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD_SKILL_TC006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD_SKILL_TC007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD_SKILL_TC008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error path: Insert an skill name without the name field
+- “Required” error text pop out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD_SKILL_TC009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD_SKILL_TC010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error path: Insert an skill name with too long name
+- “Should not exceed 120 characters” error text pop out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD_SKILL_TC011</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Error path: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Insert an skill name and description with too long content
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- “Should not exceed 120 characters” error text pop out on Skill name field
+- “Should not exceed 400 characters” error text pop out on Description field</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD_SKILL_TC012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error path: Insert an empty skill name and too long description
+- “Required” error text pop out on Skill name field
+- “Should not exceed 400 characters” error text pop out on Description field</t>
   </si>
 </sst>
 </file>
@@ -105,7 +247,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -126,6 +268,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -196,18 +343,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="55.29"/>
   </cols>
   <sheetData>
@@ -410,6 +557,23 @@
       </c>
       <c r="E12" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -421,4 +585,258 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="63.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.03"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>